<commit_message>
fix error + adding printout function
</commit_message>
<xml_diff>
--- a/data/h모의고사/h모의고사 정답 및 배점.xlsx
+++ b/data/h모의고사/h모의고사 정답 및 배점.xlsx
@@ -7,8 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="문항 정답 및 배점" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="문항 정답 및 배점" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -414,24 +413,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>